<commit_message>
update lab 3 4
</commit_message>
<xml_diff>
--- a/lab3/Описание моделей.xlsx
+++ b/lab3/Описание моделей.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\bmstu_labs\data-base-labs\lab3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\БД\data-base-labs\lab3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{366F275D-5117-4C13-A146-07DB54F2BB51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259D7EFF-CBBE-4562-B3F3-E446F6618041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Описание структуры таблиц" sheetId="1" r:id="rId1"/>
-    <sheet name="Список всех связей" sheetId="3" r:id="rId2"/>
-    <sheet name="Правила изменений" sheetId="2" r:id="rId3"/>
+    <sheet name="Ограничения мин. Кардинальности" sheetId="2" r:id="rId2"/>
+    <sheet name="Список всех связей" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="151">
   <si>
     <t>Column Name</t>
   </si>
@@ -137,9 +137,6 @@
     <t>PartnerID</t>
   </si>
   <si>
-    <t>Уникальный ключ (AK7.1)</t>
-  </si>
-  <si>
     <t>Хардатон</t>
   </si>
   <si>
@@ -236,9 +233,6 @@
     <t xml:space="preserve">FK </t>
   </si>
   <si>
-    <t>NULL будет обзначать, что у команды нет девиза</t>
-  </si>
-  <si>
     <t>Участник</t>
   </si>
   <si>
@@ -272,18 +266,12 @@
     <t>CHAR (10)</t>
   </si>
   <si>
-    <t>Уникальный ключ AK5.1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Суррогатный ключ </t>
   </si>
   <si>
     <t>Внешний ключ, отсылающий к отношению "Участник" (ParticipantID). Реализует связь "Капитан команды"</t>
   </si>
   <si>
-    <t>Уникальный ключ AK6.1</t>
-  </si>
-  <si>
     <t>NULL будет означать, что участник не студент МГТУ им. Н.Э. Баумана</t>
   </si>
   <si>
@@ -302,21 +290,12 @@
     <t>Внешний ключ, показывающий какая команда реализовала данный проект</t>
   </si>
   <si>
-    <t>Уникальный ключ AK4.1</t>
-  </si>
-  <si>
     <t>NULL будет означать, что команда, реализовавшая проект либо не может предоставить фото, либо не желает этого делать</t>
   </si>
   <si>
     <t xml:space="preserve">Операция </t>
   </si>
   <si>
-    <t>Действие над родительской таблицей</t>
-  </si>
-  <si>
-    <t>Действие над дочерней таблицей</t>
-  </si>
-  <si>
     <t>Вставка</t>
   </si>
   <si>
@@ -401,19 +380,10 @@
     <t>o-o</t>
   </si>
   <si>
-    <t>Изменение главного или внешнего ключа</t>
-  </si>
-  <si>
     <t>Подбор родительской записи "Мероприятие"</t>
   </si>
   <si>
-    <t>Ничего не требуется</t>
-  </si>
-  <si>
     <t>Подбор родительской записи "Партнёр"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Каскадное обновление </t>
   </si>
   <si>
     <t>Запрещено</t>
@@ -473,10 +443,64 @@
     <t>Внешний ключ, связывающий участника с его активной командой. NULL в этом контесте означает отсутсивте активной команды у участника</t>
   </si>
   <si>
-    <t>Разрешено, но участники должны выбрать новую команду, после удаления команда всех бывших участников станет  NULL</t>
-  </si>
-  <si>
-    <t>Разрешено, только если капитан не единсвтенный участник команды</t>
+    <t>Без ограничения</t>
+  </si>
+  <si>
+    <t>Запрет</t>
+  </si>
+  <si>
+    <t>Действие над родительской таблицей "Команда"</t>
+  </si>
+  <si>
+    <t>Действие над дочерней таблицей "Участник"</t>
+  </si>
+  <si>
+    <t>Без ограничений</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Проект создан на хардатоне		</t>
+  </si>
+  <si>
+    <t>Действие над дочерней таблицей "Команда_Мероприятия"</t>
+  </si>
+  <si>
+    <t>Изменение</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Действие над родительской таблицей "Хардтон" </t>
+  </si>
+  <si>
+    <t>Действие над дочерней таблицей "Проект"</t>
+  </si>
+  <si>
+    <t>Разрешено, если новое значение внешнего ключа соответсвует некоторому значению в родительской  таблице "Хардтон".</t>
+  </si>
+  <si>
+    <t>Разрешено, если новое значение внешнего ключа соответсвует некоторому значению в родительской таблице  "Команда".</t>
+  </si>
+  <si>
+    <t>Действие над родительской таблицей "Классическое мероприятие"</t>
+  </si>
+  <si>
+    <t>Разрешено, удаление совершается Капитаном команды, после удаления у всех участников внешний ключ становится равным NULL. Команда так же удаляется, если в ней осталось 0 участников.</t>
+  </si>
+  <si>
+    <t>Действие над родительской  таблицей "Команда"</t>
+  </si>
+  <si>
+    <t>Разрешено, если капитан, не единсвтенный участник команды, то новым капитаном становиться случайный участник команды. Если же команда состоит только из капитана, она удаляется при удалении капитана</t>
+  </si>
+  <si>
+    <t>CHAR (300)</t>
+  </si>
+  <si>
+    <t>Уникальный ключ AK1.1</t>
+  </si>
+  <si>
+    <t>CHAR (200)</t>
+  </si>
+  <si>
+    <t>NULL будет обозначать, что у команды нет девиза</t>
   </si>
 </sst>
 </file>
@@ -837,25 +861,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -874,9 +894,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -918,13 +935,16 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1058,6 +1078,44 @@
         <charset val="204"/>
         <scheme val="major"/>
       </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="major"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="major"/>
+      </font>
       <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1177,34 +1235,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri Light"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="major"/>
-      </font>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri Light"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="major"/>
-      </font>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2811,20 +2841,6 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{C6504BB5-E114-44AE-90B3-6FD1F22353C0}" name="Таблица11" displayName="Таблица11" ref="A1:E9" totalsRowShown="0" dataDxfId="45">
-  <autoFilter ref="A1:E9" xr:uid="{C6504BB5-E114-44AE-90B3-6FD1F22353C0}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{1AB3F472-F101-4165-AE9F-BCF6DDAF7847}" name="Родительская таблица" dataDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{0B1EF4C9-F326-4022-834D-4FAFFFC1C93A}" name="Дочерняя таблица" dataDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{0484B746-4CDA-4B2E-BFA4-8B4308109CC2}" name="Название " dataDxfId="42"/>
-    <tableColumn id="4" xr3:uid="{00A6F6C0-8E75-4C39-BE5C-118A2E667956}" name="Тип связи " dataDxfId="41"/>
-    <tableColumn id="5" xr3:uid="{639BCF4F-57EF-42C9-98C8-D78C4F20E71C}" name="Связь" dataDxfId="40"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{5BA4DB45-8CBC-45B1-B670-EFD20862F9CE}" name="Таблица12" displayName="Таблица12" ref="A2:C5" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
   <autoFilter ref="A2:C5" xr:uid="{5BA4DB45-8CBC-45B1-B670-EFD20862F9CE}"/>
   <tableColumns count="3">
@@ -2836,7 +2852,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{62ACB0E3-641F-47FA-BD4F-B7681477F454}" name="Таблица1214" displayName="Таблица1214" ref="E2:G5" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
   <autoFilter ref="E2:G5" xr:uid="{62ACB0E3-641F-47FA-BD4F-B7681477F454}"/>
   <tableColumns count="3">
@@ -2848,73 +2864,87 @@
 </table>
 </file>
 
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{EA31F29F-C6EF-4101-A4C0-9224A1137D68}" name="Таблица1216" displayName="Таблица1216" ref="A8:C11" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
   <autoFilter ref="A8:C11" xr:uid="{EA31F29F-C6EF-4101-A4C0-9224A1137D68}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{A0E1DAD7-B71D-4707-82CD-755EE3135B20}" name="Операция " dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{6C146020-7822-4DEF-9A71-C21F462173D0}" name="Действие над родительской таблицей" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{84F4FFF8-C098-4492-BFA0-CBAD79D6B412}" name="Действие над дочерней таблицей" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{6C146020-7822-4DEF-9A71-C21F462173D0}" name="Действие над родительской таблицей &quot;Хардтон&quot; " dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{84F4FFF8-C098-4492-BFA0-CBAD79D6B412}" name="Действие над дочерней таблицей &quot;Проект&quot;" dataDxfId="25"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{74ED1DCB-1224-42A9-9BE2-D8C4C566DA94}" name="Таблица121617" displayName="Таблица121617" ref="E8:G11" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+  <autoFilter ref="E8:G11" xr:uid="{74ED1DCB-1224-42A9-9BE2-D8C4C566DA94}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{DC232AB2-1A8A-46F6-826C-C41D72BF6521}" name="Операция " dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{3ECE36ED-FB9C-4E27-8CE4-34D78B0F2FB9}" name="Действие над родительской таблицей &quot;Классическое мероприятие&quot;" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{12D67879-9503-495F-B01E-943D2F23BB75}" name="Действие над дочерней таблицей &quot;Команда_Мероприятия&quot;" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{74ED1DCB-1224-42A9-9BE2-D8C4C566DA94}" name="Таблица121617" displayName="Таблица121617" ref="E8:G11" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
-  <autoFilter ref="E8:G11" xr:uid="{74ED1DCB-1224-42A9-9BE2-D8C4C566DA94}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{8A7AA15D-871F-4A54-A759-3349A8637A74}" name="Таблица12161718" displayName="Таблица12161718" ref="E14:G17" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="E14:G17" xr:uid="{8A7AA15D-871F-4A54-A759-3349A8637A74}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{DC232AB2-1A8A-46F6-826C-C41D72BF6521}" name="Операция " dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{3ECE36ED-FB9C-4E27-8CE4-34D78B0F2FB9}" name="Действие над родительской таблицей" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{12D67879-9503-495F-B01E-943D2F23BB75}" name="Действие над дочерней таблицей" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{D088C6AB-2FF0-4150-AFC4-49D652038259}" name="Операция " dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{69179C73-05B4-4063-9C63-5A91D2B9D3FD}" name="Действие над родительской таблицей &quot;Команда&quot;" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{27289A53-EBAB-410C-BD36-81ADA3ED179E}" name="Действие над дочерней таблицей &quot;Команда_Мероприятия&quot;" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{8A7AA15D-871F-4A54-A759-3349A8637A74}" name="Таблица12161718" displayName="Таблица12161718" ref="E14:G17" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="E14:G17" xr:uid="{8A7AA15D-871F-4A54-A759-3349A8637A74}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{75A08EF5-3ACC-4937-B26F-9CF4F5C8FC90}" name="Таблица1216171819" displayName="Таблица1216171819" ref="A14:C17" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+  <autoFilter ref="A14:C17" xr:uid="{75A08EF5-3ACC-4937-B26F-9CF4F5C8FC90}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{D088C6AB-2FF0-4150-AFC4-49D652038259}" name="Операция " dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{69179C73-05B4-4063-9C63-5A91D2B9D3FD}" name="Действие над родительской таблицей" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{27289A53-EBAB-410C-BD36-81ADA3ED179E}" name="Действие над дочерней таблицей" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{0CDA3B41-3662-4B75-B3B0-38D439ABA363}" name="Операция " dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{54335295-F20F-41B9-9FED-1BB09BB2D50F}" name="Действие над родительской таблицей &quot;Команда&quot;" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{2AC780B6-A3D8-494E-A671-56D05AC8BD65}" name="Действие над дочерней таблицей &quot;Участник&quot;" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{75A08EF5-3ACC-4937-B26F-9CF4F5C8FC90}" name="Таблица1216171819" displayName="Таблица1216171819" ref="A14:C17" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="A14:C17" xr:uid="{75A08EF5-3ACC-4937-B26F-9CF4F5C8FC90}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{26719D3F-4CEB-4E22-93FF-F4226F3B24BC}" name="Таблица121617181920" displayName="Таблица121617181920" ref="A20:C23" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A20:C23" xr:uid="{26719D3F-4CEB-4E22-93FF-F4226F3B24BC}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{0CDA3B41-3662-4B75-B3B0-38D439ABA363}" name="Операция " dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{54335295-F20F-41B9-9FED-1BB09BB2D50F}" name="Действие над родительской таблицей" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{2AC780B6-A3D8-494E-A671-56D05AC8BD65}" name="Действие над дочерней таблицей" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{9DEE324A-7951-4878-AE78-320B65819691}" name="Операция " dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{F8C87BC2-B345-4864-B086-08223059526A}" name="Действие над родительской  таблицей &quot;Команда&quot;" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{71221CD6-A78B-4CF4-B664-0BD8AC3ADD4B}" name="Действие над дочерней таблицей &quot;Участник&quot;" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{26719D3F-4CEB-4E22-93FF-F4226F3B24BC}" name="Таблица121617181920" displayName="Таблица121617181920" ref="A20:C23" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A20:C23" xr:uid="{26719D3F-4CEB-4E22-93FF-F4226F3B24BC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{B59E590C-E96E-41B0-9E5C-C10C82D415C9}" name="Таблица12161718192021" displayName="Таблица12161718192021" ref="E20:G23" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="E20:G23" xr:uid="{B59E590C-E96E-41B0-9E5C-C10C82D415C9}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{9DEE324A-7951-4878-AE78-320B65819691}" name="Операция " dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{F8C87BC2-B345-4864-B086-08223059526A}" name="Действие над родительской таблицей" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{71221CD6-A78B-4CF4-B664-0BD8AC3ADD4B}" name="Действие над дочерней таблицей" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{3B0CBF4B-C263-402C-B44D-D3666B74E6DE}" name="Операция " dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{D3479BE3-4AA8-403D-B20B-352507DDA74C}" name="Действие над родительской таблицей &quot;Команда&quot;" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{559BF620-9853-472A-B8BC-53A63F0D1AFC}" name="Действие над дочерней таблицей &quot;Проект&quot;" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{B59E590C-E96E-41B0-9E5C-C10C82D415C9}" name="Таблица12161718192021" displayName="Таблица12161718192021" ref="E20:G23" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="E20:G23" xr:uid="{B59E590C-E96E-41B0-9E5C-C10C82D415C9}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{3B0CBF4B-C263-402C-B44D-D3666B74E6DE}" name="Операция " dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{D3479BE3-4AA8-403D-B20B-352507DDA74C}" name="Действие над родительской таблицей" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{559BF620-9853-472A-B8BC-53A63F0D1AFC}" name="Действие над дочерней таблицей" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{C6504BB5-E114-44AE-90B3-6FD1F22353C0}" name="Таблица11" displayName="Таблица11" ref="A1:E9" totalsRowShown="0" dataDxfId="45">
+  <autoFilter ref="A1:E9" xr:uid="{C6504BB5-E114-44AE-90B3-6FD1F22353C0}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{1AB3F472-F101-4165-AE9F-BCF6DDAF7847}" name="Родительская таблица" dataDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{0B1EF4C9-F326-4022-834D-4FAFFFC1C93A}" name="Дочерняя таблица" dataDxfId="43"/>
+    <tableColumn id="3" xr3:uid="{0484B746-4CDA-4B2E-BFA4-8B4308109CC2}" name="Название " dataDxfId="42"/>
+    <tableColumn id="4" xr3:uid="{00A6F6C0-8E75-4C39-BE5C-118A2E667956}" name="Тип связи " dataDxfId="41"/>
+    <tableColumn id="5" xr3:uid="{639BCF4F-57EF-42C9-98C8-D78C4F20E71C}" name="Связь" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3297,927 +3327,926 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.44140625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" style="12" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" style="12" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" style="12" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" style="12" customWidth="1"/>
-    <col min="6" max="6" width="16.109375" style="12" customWidth="1"/>
-    <col min="7" max="7" width="22.44140625" style="12" customWidth="1"/>
-    <col min="8" max="8" width="12" style="12" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" style="12" customWidth="1"/>
-    <col min="10" max="10" width="13.88671875" style="12" customWidth="1"/>
-    <col min="11" max="11" width="16.88671875" style="12" customWidth="1"/>
-    <col min="12" max="13" width="9.109375" style="12"/>
-    <col min="14" max="14" width="15.6640625" style="12" customWidth="1"/>
-    <col min="15" max="15" width="13" style="12" customWidth="1"/>
-    <col min="16" max="16" width="15.88671875" style="12" customWidth="1"/>
-    <col min="17" max="17" width="13.88671875" style="12" customWidth="1"/>
-    <col min="18" max="18" width="20.109375" style="12" customWidth="1"/>
-    <col min="19" max="16384" width="9.109375" style="12"/>
+    <col min="1" max="1" width="30.42578125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" style="10" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" style="10" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" style="10" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" style="10" customWidth="1"/>
+    <col min="8" max="8" width="12" style="10" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" style="10" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" style="10" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" style="10" customWidth="1"/>
+    <col min="12" max="13" width="9.140625" style="10"/>
+    <col min="14" max="14" width="15.7109375" style="10" customWidth="1"/>
+    <col min="15" max="15" width="13" style="10" customWidth="1"/>
+    <col min="16" max="16" width="15.85546875" style="10" customWidth="1"/>
+    <col min="17" max="17" width="13.85546875" style="10" customWidth="1"/>
+    <col min="18" max="18" width="20.140625" style="10" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
-        <v>136</v>
-      </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="39"/>
-      <c r="G1" s="31" t="s">
+    <row r="1" spans="1:18" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="37"/>
+      <c r="G1" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="31"/>
+      <c r="N1" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="31"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="R2" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="33"/>
-      <c r="N1" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="33"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
+      <c r="N3" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q3" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="R3" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="P4" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="R4" s="16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="O5" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="P5" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q5" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="R5" s="12"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="N6" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="O6" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="P6" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q6" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="R6" s="23"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="31"/>
+      <c r="G13" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="31"/>
+      <c r="N13" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="O13" s="30"/>
+      <c r="P13" s="30"/>
+      <c r="Q13" s="30"/>
+      <c r="R13" s="31"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B14" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C14" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D14" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E14" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="F14" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H14" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="I14" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="J14" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="K14" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="N2" s="16" t="s">
+      <c r="N14" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="O2" s="17" t="s">
+      <c r="O14" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="P2" s="17" t="s">
+      <c r="P14" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="17" t="s">
+      <c r="Q14" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="18" t="s">
+      <c r="R14" s="15" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+    <row r="15" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B15" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C15" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="G15" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="J15" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="K15" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="N15" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="O15" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="P15" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="Q15" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="13" t="s">
+      <c r="R15" s="16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="105" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="H16" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="I16" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="J16" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="K16" s="23"/>
+      <c r="N16" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="O16" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="P16" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q16" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="R16" s="16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="N17" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="O17" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="P17" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q17" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="R17" s="16" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="90" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="K18" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="L18" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="M18" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="N18" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="O18" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="P18" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q18" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="R18" s="16" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="120" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="L19" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="N19" s="19"/>
+      <c r="O19" s="20"/>
+      <c r="P19" s="20"/>
+      <c r="Q19" s="20"/>
+      <c r="R19" s="23"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" s="30"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="31"/>
+      <c r="G22" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="31"/>
+      <c r="N22" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="O22" s="33"/>
+      <c r="P22" s="33"/>
+      <c r="Q22" s="33"/>
+      <c r="R22" s="34"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="I23" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="J23" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="K23" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="N23" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="O23" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="P23" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q23" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="R23" s="14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I24" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="J24" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K24" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="N24" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="O24" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="P24" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q24" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="R24" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="135" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="G25" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="H25" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="20" t="s">
+      <c r="I25" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="J25" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="K25" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="N25" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="O25" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="P25" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q25" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="R25" s="25" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="N26" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="O26" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="P26" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q26" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="R26" s="25" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="N27" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="O27" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="P27" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q27" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="75" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="12"/>
+      <c r="N28" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="O28" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="P28" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q28" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="R28" s="25" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="120" x14ac:dyDescent="0.25">
+      <c r="A29" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D29" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="N29" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="O29" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="P29" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q29" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="J3" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="K3" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="N3" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="O3" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="P3" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q3" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="R3" s="21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="H4" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="J4" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="N4" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="O4" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="P4" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q4" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="R4" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="N5" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="O5" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="P5" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q5" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="R5" s="15"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="N6" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="O6" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="P6" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q6" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="R6" s="26"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="24" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="33"/>
-      <c r="G13" s="31" t="s">
-        <v>54</v>
-      </c>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="33"/>
-      <c r="N13" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="O13" s="32"/>
-      <c r="P13" s="32"/>
-      <c r="Q13" s="32"/>
-      <c r="R13" s="33"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="G14" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="H14" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="I14" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="J14" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="K14" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="N14" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="O14" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="P14" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q14" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="R14" s="18" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="G15" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="H15" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="I15" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="J15" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="K15" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="N15" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="O15" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="P15" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q15" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="R15" s="19" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="G16" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="H16" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="I16" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="J16" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="K16" s="26"/>
-      <c r="N16" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="O16" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="P16" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q16" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="R16" s="19" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="N17" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="O17" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="P17" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q17" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="R17" s="19" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A18" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="E18" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="K18" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="L18" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="M18" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="N18" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="O18" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="P18" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q18" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="R18" s="19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="E19" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="L19" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="N19" s="22"/>
-      <c r="O19" s="23"/>
-      <c r="P19" s="23"/>
-      <c r="Q19" s="23"/>
-      <c r="R19" s="26"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" s="22" t="s">
+      <c r="R29" s="25" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E32" s="10" t="s">
         <v>43</v>
-      </c>
-      <c r="B20" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A22" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="B22" s="32"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="33"/>
-      <c r="G22" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="H22" s="32"/>
-      <c r="I22" s="32"/>
-      <c r="J22" s="32"/>
-      <c r="K22" s="33"/>
-      <c r="N22" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="O22" s="35"/>
-      <c r="P22" s="35"/>
-      <c r="Q22" s="35"/>
-      <c r="R22" s="36"/>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A23" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E23" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="G23" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="H23" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="I23" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="J23" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="K23" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="N23" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="O23" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="P23" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q23" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="R23" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="G24" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="H24" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I24" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="J24" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="K24" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="N24" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="O24" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="P24" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q24" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="R24" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A25" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="G25" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="H25" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="I25" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="J25" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="K25" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="N25" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="O25" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="P25" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q25" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="R25" s="28" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="B26" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E26" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="F26" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="N26" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="O26" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="P26" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q26" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="R26" s="28" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A27" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="N27" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="O27" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="P27" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q27" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="R27" s="14"/>
-    </row>
-    <row r="28" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D28" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E28" s="15"/>
-      <c r="N28" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="O28" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="P28" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q28" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="R28" s="28" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="B29" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="D29" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="E29" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="G29" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="N29" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="O29" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="P29" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q29" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="R29" s="28" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="E32" s="12" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -4249,569 +4278,391 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B57C1CDE-30ED-4CFF-9BF7-9700AC224619}">
-  <dimension ref="A1:E9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="23.109375" customWidth="1"/>
-    <col min="3" max="3" width="22.5546875" customWidth="1"/>
-    <col min="4" max="4" width="28" customWidth="1"/>
-    <col min="5" max="5" width="22.44140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="30" t="s">
-        <v>102</v>
-      </c>
-      <c r="B2" s="30" t="s">
-        <v>103</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D2" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="E2" s="30" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="30" t="s">
-        <v>103</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D3" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="E3" s="30" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D4" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="E4" s="30" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" s="30" t="s">
-        <v>104</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D5" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="E5" s="30" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="B6" s="30" t="s">
-        <v>106</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D6" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="E6" s="30" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="B7" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D7" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="E7" s="30" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D8" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="E8" s="30" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="B9" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D9" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="E9" s="30" t="s">
-        <v>122</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{862677DE-292B-40BB-B576-5DF72EB5AC99}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" style="2" customWidth="1"/>
-    <col min="2" max="2" width="38.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="34.44140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" style="2"/>
-    <col min="5" max="5" width="14" style="2" customWidth="1"/>
-    <col min="6" max="6" width="36.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="34" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9.109375" style="2"/>
+    <col min="1" max="1" width="14" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="14" style="1" customWidth="1"/>
+    <col min="6" max="6" width="43" style="1" customWidth="1"/>
+    <col min="7" max="7" width="38.140625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="40" t="s">
-        <v>98</v>
-      </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="42"/>
-      <c r="E1" s="40" t="s">
-        <v>110</v>
-      </c>
-      <c r="F1" s="41"/>
-      <c r="G1" s="42"/>
-    </row>
-    <row r="2" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B2" s="4" t="s">
+    <row r="1" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="40"/>
+      <c r="E1" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="39"/>
+      <c r="G1" s="40"/>
+    </row>
+    <row r="2" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C4" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="38" t="s">
+        <v>136</v>
+      </c>
+      <c r="B7" s="39"/>
+      <c r="C7" s="40"/>
+      <c r="E7" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" s="39"/>
+      <c r="G7" s="40"/>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13" s="39"/>
+      <c r="C13" s="40"/>
+      <c r="E13" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="F13" s="39"/>
+      <c r="G13" s="40"/>
+    </row>
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="F2" s="4" t="s">
+      <c r="E14" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G14" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" s="39"/>
+      <c r="C19" s="40"/>
+      <c r="E19" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="F19" s="39"/>
+      <c r="G19" s="40"/>
+    </row>
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="B4" s="7" t="s">
+      <c r="E20" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="F4" s="7" t="s">
+      <c r="E21" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G21" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="40" t="s">
-        <v>112</v>
-      </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="42"/>
-      <c r="E7" s="40" t="s">
-        <v>113</v>
-      </c>
-      <c r="F7" s="41"/>
-      <c r="G7" s="42"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="C9" s="8" t="s">
+    </row>
+    <row r="22" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B22" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="G23" s="9" t="s">
         <v>135</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="40" t="s">
-        <v>114</v>
-      </c>
-      <c r="B13" s="41"/>
-      <c r="C13" s="42"/>
-      <c r="E13" s="40" t="s">
-        <v>111</v>
-      </c>
-      <c r="F13" s="41"/>
-      <c r="G13" s="42"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="40" t="s">
-        <v>115</v>
-      </c>
-      <c r="B19" s="41"/>
-      <c r="C19" s="42"/>
-      <c r="E19" s="40" t="s">
-        <v>116</v>
-      </c>
-      <c r="F19" s="41"/>
-      <c r="G19" s="42"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="G23" s="11" t="s">
-        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -4838,4 +4689,182 @@
     <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B57C1CDE-30ED-4CFF-9BF7-9700AC224619}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" customWidth="1"/>
+    <col min="4" max="4" width="28" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>